<commit_message>
fix bux by starting waitclock earlier
</commit_message>
<xml_diff>
--- a/output_files/vote-on-super-popular-after-wait/sm_50/500-epochs.xlsx
+++ b/output_files/vote-on-super-popular-after-wait/sm_50/500-epochs.xlsx
@@ -392,22 +392,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="n">
-        <v>807.4802320404739</v>
+        <v>807.6077450938764</v>
       </c>
       <c r="B2" t="n">
-        <v>21166.75412334597</v>
+        <v>1156.06823400084</v>
       </c>
       <c r="C2" t="n">
-        <v>35142.49365176656</v>
+        <v>2076.469173250837</v>
       </c>
       <c r="D2" t="n">
-        <v>70129.67417061611</v>
+        <v>6478.50722779852</v>
       </c>
       <c r="E2" t="n">
-        <v>109109.0172765462</v>
+        <v>16215.62762482892</v>
       </c>
       <c r="F2" t="n">
-        <v>276368.7134646963</v>
+        <v>51584.20364845017</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -415,19 +415,19 @@
         <v>8.986000000000001</v>
       </c>
       <c r="B3" t="n">
-        <v>8.638984760300907</v>
+        <v>9.001688094533295</v>
       </c>
       <c r="C3" t="n">
-        <v>60.4491182822111</v>
+        <v>8.845335456611505</v>
       </c>
       <c r="D3" t="n">
-        <v>28.06025221389988</v>
+        <v>8.609078161932615</v>
       </c>
       <c r="E3" t="n">
-        <v>20.14457452420566</v>
+        <v>8.801139489036734</v>
       </c>
       <c r="F3" t="n">
-        <v>24.55740072202166</v>
+        <v>10.39958739790717</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -455,19 +455,19 @@
         <v>0.998000799680128</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1389244302279088</v>
+        <v>0.8620551779288285</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07277089164334266</v>
+        <v>0.6441423430627748</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05853658536585366</v>
+        <v>0.3682327069172331</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05651739304278289</v>
+        <v>0.2402838864454218</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04618152738904438</v>
+        <v>0.1462215113954418</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -475,19 +475,19 @@
         <v>0.001995983984032128</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0004099200655872105</v>
+        <v>0.00172229409573552</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0005466213335374053</v>
+        <v>0.001287409059188732</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0003625690607734807</v>
+        <v>0.0007352468500899975</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0002773944340806802</v>
+        <v>0.0004788693853570595</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0002174673562588051</v>
+        <v>0.0002902348080217676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>